<commit_message>
Dossier excel bien avancé + Site web presque terminé
</commit_message>
<xml_diff>
--- a/annexe/aymeric-audit-SEO.xlsx
+++ b/annexe/aymeric-audit-SEO.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="157">
   <si>
     <t>Catégorie</t>
   </si>
@@ -81,30 +81,6 @@
   Si votre région possède un journal digital, n'hésitez pas à envoyer un email pour vous présenter. </t>
   </si>
   <si>
-    <r>
-      <t>Il est très important d'</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>encourager les avis favorables</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t> et de répondre aux avis négatifs. Vérifiez sur les plateformes d'avis que vous n'avez pas un compte créé d'office, ce qui est une pratique courante.</t>
-    </r>
-  </si>
-  <si>
     <t>Lier votre site web à une plateforme/site d'avis comme :  Tripadvisior, Yelp, Glassdoor ou Truspilot.</t>
   </si>
   <si>
@@ -127,58 +103,10 @@
     <t>Vérifiez si le site a une version principale (www ou non www)</t>
   </si>
   <si>
-    <r>
-      <t>Une URL de site peut être écrite avec ou sans "www". Ceci n'a pas d'importance au niveau du SEO s'il existe une version principale et qu'elle est </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>bien paramétrée</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t> ! Il ne faut surtout pas avoir deux fois le même site en www et sans www</t>
-    </r>
-  </si>
-  <si>
     <t>La bonne pratique consiste à choisir l'une des deux puis de rediriger celle qui n'est pas utilisée grâce à une redirection 301.</t>
   </si>
   <si>
     <t>Vérifiez que le site n'a pas de contenu dupliqué</t>
-  </si>
-  <si>
-    <r>
-      <t>Des pages d'un site web ayant du contenu copier-coller ou très similaire sont ce qu'on appelle du "</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>contenu dupliqué</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>". Ce contenu se trouve souvent sur des pages produits similaires ou des pages d'archive ou de catégorie. Il se peut aussi que votre organisation ou client ait copié-collé des pages locales, en ne changeant que le nom de la ville par exemple.</t>
-    </r>
   </si>
   <si>
     <t>Prenez  le temps de vérifier quelques-unes de ces pages à la main. Vous pouvez aussi utiliser un site comme Siteliner, qui repère les problèmes de plagiat automatiquement.</t>
@@ -200,271 +128,24 @@
     <t>Balise TITLE et DESCRIPTION</t>
   </si>
   <si>
-    <r>
-      <t>ces balises indiquent aux moteurs de recherche de quoi traite la page. Elles sont aussi affichées dans les résultats. Elles doivent donc non seulement </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>contenir le mot-clé</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t> visé, mais aussi </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>donner envie</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t> au visiteur de cliquer pour lire votre page.</t>
-    </r>
-  </si>
-  <si>
     <t>Balise ROBOT</t>
   </si>
   <si>
-    <r>
-      <t>vérifiez que le contenu de cette balise est bien en "index, follow". Cela indique aux moteurs de recherche qu'ils doivent </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>indexer la page</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t> (index) et </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>suivre les liens</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t> présents sur celle-ci (follow).</t>
-    </r>
-  </si>
-  <si>
     <t>Titres</t>
   </si>
   <si>
-    <r>
-      <t>Vérifiez qu'il n'y a qu'</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>un et un seul h1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t> sur la page, et qu'il contient le mot-clé ;
-Vérifiez que le contenu est segmenté en plusieurs sous-parties par des h2 et qu'ils contiennent soit le mot-clé, soit un synonyme proche.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Les </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>images ne doivent pas être trop lourdes</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>. Si une image est censée être de petite taille sur le site, il ne faut absolument pas y insérer une grande image et laisser le code faire l'adaptation de taille. En effet, plus l'image est grande, plus elle prend du temps à télécharger.</t>
-    </r>
-  </si>
-  <si>
     <t>Tailles des images</t>
   </si>
   <si>
     <t>Images : balises ALT</t>
   </si>
   <si>
-    <r>
-      <t>Vérifiez également que toutes les images contiennent </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>des balises "alt"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t> écrites de cette manière : 
-&lt;img src="https://monsite.com/image.png" alt="Description de l'image" /&gt;
-Cette balise sert à expliquer le contenu de l'image aux moteurs de recherche et s'affiche quand les images ne peuvent être chargées. Elle sert aussi à décrire l'image pour les personnes malvoyantes. Il est donc conseillé de décrire correctement l'image et si possible, d'y ajouter le mot-clé.</t>
-    </r>
-  </si>
-  <si>
     <t>Cohérence et longueur du contenu</t>
   </si>
   <si>
-    <r>
-      <t>Il était auparavant conseillé d'écrire un minimum de 250 mots sur une page. De nos jours, il existe très peu de pages en première position avec si peu de contenu. Visez grand </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>minimum 400 mots</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t> pour les pages de votre site (lorsque c'est cohérent) et 600 mots pour vos articles de blog, vos pages d'expertise ou d'actualités. </t>
-    </r>
-  </si>
-  <si>
     <t>Examinez les positions de vos mots-clés</t>
   </si>
   <si>
-    <r>
-      <t>Vérifier, à l'aide de google analytics,  que l'</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>évolution du trafic</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t> va dans le bon sens. En effet, le trafic organique de votre site est censé </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>augmenter</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t> ou, au moins, rester </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>stable</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>. Cette étape vous servira également à comprendre sur quels mots-clés votre site remonte avant toute modification SEO. Cela pourra peut-être vous donner des idées de mots-clés que vous auriez oubliés.</t>
-    </r>
-  </si>
-  <si>
     <t>Vérifiez la qualité des liens existants</t>
   </si>
   <si>
@@ -480,57 +161,7 @@
     <t xml:space="preserve">Focalisez vous sur un seul sujet par page, et sructure correctement vos pages. </t>
   </si>
   <si>
-    <r>
-      <t>Chaque page ne traite que d'</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>un seul sujet,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> c'est à dire qu'elle ne contient qu'un mot clé principal. Ce mot clé doit absolument figurer dans l'URL de la page. Toutes les pages de votre site doivent avoir un seul titre h1, plusieurs h2, au moins 1 image, plusieurs paragaraphe, quelques liens interne et externe. 
-Les pages doivent être liées entre elles de manière cohérente. 
-</t>
-    </r>
-  </si>
-  <si>
     <t>Créez votre machine à contenu</t>
-  </si>
-  <si>
-    <r>
-      <t>Plus vous créerez de contenu de qualité, plus vous aurez de pages indexées par Google et donc de </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>portes d'entrées potentielles</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> pour vos visiteurs. Il est donc nécessaire de créer un espace dédié à acceuillir ce contenu. </t>
-    </r>
   </si>
   <si>
     <t xml:space="preserve">Définissez votre type de contenu(articles intéressants, fiches de postes, actualités, article sur votre expertise etc…) et mettez votre site régulièrement à jour. </t>
@@ -673,83 +304,6 @@
   </si>
   <si>
     <t>Revoir certaines URL</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">les URLs du site ne </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>sont pas intelligibles</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Remplacez les URLs impossibles à lire,</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>par exemple</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t> "https://monsite.com/345e93", par :</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> "</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>https://monsite.com/mot-cle-principal</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>" !</t>
-    </r>
   </si>
   <si>
     <t>Adaptez la taille des images avant insertion.</t>
@@ -812,15 +366,9 @@
     <t>Voir wave et TPGi’s  color contrast checker tool</t>
   </si>
   <si>
-    <t>c'est surtout a couleur orange  qui pose problème</t>
-  </si>
-  <si>
     <t>La structure de la page n'est pas idéale</t>
   </si>
   <si>
-    <t>Voir heading map</t>
-  </si>
-  <si>
     <t>Les descriptions des images ne sont pas adaptées</t>
   </si>
   <si>
@@ -877,6 +425,570 @@
         <family val="2"/>
       </rPr>
       <t>est un langage de code créé spécifiquement pour prendre en charge l'accessibilité. ARIA vous permet de créer des composants personnalisés dont l'apparence et le comportement sont conformes à vos souhaits, puis d'identifier leur fonction et leur état.</t>
+    </r>
+  </si>
+  <si>
+    <t>Note pour Aymeric</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A faire à la fin </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Placez du texte sous forme d'image ne permet pas de valoriser les mots clés et donc d'optimiser le référencement. De plus, le texte s'adapte plus facilement que l'image au responsive. </t>
+  </si>
+  <si>
+    <t>Image à la place d'un texte.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Absence de label dans le formulaire </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Si un formulaire n'a pas de label associé, sa fonction n'est pas reconnu par les utilisateurs de lecteur d'écran. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Assiocier à chaque formulaire un label. </t>
+  </si>
+  <si>
+    <t>Balise meta keywords inutile</t>
+  </si>
+  <si>
+    <t>Le moteur de recherche google ne prend plus en compte cette balise. De plus, la concurrence peut avoir accès à vos mots clés.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Supprimer cette balise et mettre en valeur ses mots clés autrement. </t>
+  </si>
+  <si>
+    <t>Ajoutez une balise robot avec comme contenu "index, follow".</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Utile pour éviter des problème d'indexation avec du  duplicate content. </t>
+  </si>
+  <si>
+    <t>Balise canonique url</t>
+  </si>
+  <si>
+    <t>Ajoutez une balise canonique.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Paramétrez le cache navigateur </t>
+  </si>
+  <si>
+    <t>Un cache est un espace de stockage de données temporaire, permettant de réafficher ces données plus rapidement. La mise en cache navigateur permet d’accélérer le temps de chargement de vos pages pour vos visiteurs lorsqu’ils reviennent sur votre site.</t>
+  </si>
+  <si>
+    <t>Paramétrez le cache navigateur dans le fichier .htacces</t>
+  </si>
+  <si>
+    <t>Ajoutez un attibut async au niveau des scripts.</t>
+  </si>
+  <si>
+    <t>scripts javascript</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dans les sites Web modernes, les scripts sont souvent “plus lourds” que le HTML: leur taille de téléchargement est plus grande et le temps de traitement est également plus long.
+Lorsque le navigateur charge le HTML et rencontre une balise &lt;script&gt;...&lt;/script&gt;, il ne peut pas continuer à construire le DOM. Il doit exécuter le script de suite. Il en va de même pour les scripts externes &lt;script src ="..."&gt;&lt;/script&gt;: le navigateur doit attendre le téléchargement du script, l’exécuter, puis traiter le reste de la page.Les scripts async se chargent en arrière-plan et s’exécutent lorsqu’ils sont prêts. Cela permet donc d'augmenter la vitesse de chargement du site. </t>
+  </si>
+  <si>
+    <t>dev mozzilla, alaza creation, 3Wschool,</t>
+  </si>
+  <si>
+    <t>https://www.w3schools.com/html/html_accessibility.asp</t>
+  </si>
+  <si>
+    <t>https://developer.mozilla.org/fr/docs/Web/Accessibility/Mobile_accessibility_checklist</t>
+  </si>
+  <si>
+    <t>voir heading map</t>
+  </si>
+  <si>
+    <t>https://developers.google.com/search/docs/beginner/seo-starter-guide?hl=fr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Utilisez des mots dans les URL </t>
+  </si>
+  <si>
+    <t>https://seo-reference.net/optimisation/texte-cache.html</t>
+  </si>
+  <si>
+    <t>https://www.wearethewords.com/format-image-optimiser-seo/</t>
+  </si>
+  <si>
+    <t>https://developer.mozilla.org/en-US/docs/Web/Accessibility/ARIA</t>
+  </si>
+  <si>
+    <t>https://www.accede-web.com/notices/html-et-css/formulaires/</t>
+  </si>
+  <si>
+    <t>https://www.seo.fr/outils-seo/google-search-console</t>
+  </si>
+  <si>
+    <t>https://hugo.maugey.fr/developpeur-fullstack/minification-site-web</t>
+  </si>
+  <si>
+    <t>https://www.btobmarketers.fr/search-marketing/seo-reduire-temps-de-chargement-de-vos-pages/</t>
+  </si>
+  <si>
+    <t>https://www.kaplankomputing.com/blog/tutorials/seo/server-side-caching-seo/</t>
+  </si>
+  <si>
+    <t>https://www.w3schools.com/tags/att_script_async.asp</t>
+  </si>
+  <si>
+    <t>https://www.webrankinfo.com/dossiers/debutants/meta-keywords</t>
+  </si>
+  <si>
+    <t>https://www.accede-web.com/notices/html-et-css/formulaires/utiliser-la-balise-label-ainsi-que-les-attributs-for-et-id-pour-etiqueter-les-champs-avec-intitule-visible/</t>
+  </si>
+  <si>
+    <t>Supprimez les images et les remplacer par du texte</t>
+  </si>
+  <si>
+    <t>https://www.codeur.com/blog/seo-autorite-site-web/</t>
+  </si>
+  <si>
+    <t>https://markitors.com/keywords-for-seo/</t>
+  </si>
+  <si>
+    <t>https://www.seo.fr/definition/duplicate-content</t>
+  </si>
+  <si>
+    <t>https://www.seo.fr/guide-google-my-business</t>
+  </si>
+  <si>
+    <t>https://www.redacteur.com/blog/gestion-reputation-seo/</t>
+  </si>
+  <si>
+    <t>https://www.digitalocean.com/community/tutorials/how-to-add-twitter-card-and-open-graph-social-metadata-to-your-webpage-with-html</t>
+  </si>
+  <si>
+    <t>Optimisez votre site pour les réseaux sociaux</t>
+  </si>
+  <si>
+    <t>Améliorez la manière d'afficher vos pages sur les réseaux sociaux en indiquant plus d'informations dans les metadonnées.</t>
+  </si>
+  <si>
+    <t>Insérez les metadonnées Twitter Cards et Open Graph.</t>
+  </si>
+  <si>
+    <t>Optimisez votre logo pour le web</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Utilisez une image plutôt que du texte pour votre logo ne permet pas de valoriser votre nom de site et donc n'optimise pas votre référencement. </t>
+  </si>
+  <si>
+    <t>Les liens avec des mots pertinents pour le contenu et la structure de votre site sont plus conviviales pour les visiteurs qui consultent votre site.</t>
+  </si>
+  <si>
+    <t>Remplacez "page2" par "Contact"</t>
+  </si>
+  <si>
+    <t>Demandez à votre graphiste de vous fournir la police pour le logo du site.</t>
+  </si>
+  <si>
+    <r>
+      <t>Il est très important d'</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>encourager les avis favorables</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> et de répondre aux avis négatifs. Vérifiez sur les plateformes d'avis que vous n'avez pas un compte créé d'office, ce qui est une pratique courante.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Une URL de site peut être écrite avec ou sans "www". Ceci n'a pas d'importance au niveau du SEO s'il existe une version principale et qu'elle est </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>bien paramétrée</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> ! Il ne faut surtout pas avoir deux fois le même site en www et sans www</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Des pages d'un site web ayant du contenu copier-coller ou très similaire sont ce qu'on appelle du "</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>contenu dupliqué</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>". Ce contenu se trouve souvent sur des pages produits similaires ou des pages d'archive ou de catégorie. Il se peut aussi que votre organisation ou client ait copié-collé des pages locales, en ne changeant que le nom de la ville par exemple.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">les URLs du site ne </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>sont pas intelligibles</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Remplacez les URLs impossibles à lire,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>par exemple</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> "https://monsite.com/345e93", par :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> "</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>https://monsite.com/mot-cle-principal</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>" !</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ces balises indiquent aux moteurs de recherche de quoi traite la page. Elles sont aussi affichées dans les résultats. Elles doivent donc non seulement </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>contenir le mot-clé</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> visé, mais aussi </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>donner envie</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> au visiteur de cliquer pour lire votre page.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> La balise robot indique aux moteurs de recherche qu'ils doivent </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>indexer la page</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> (index) et </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>suivre les liens</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> présents sur celle-ci (follow).</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Vérifiez qu'il n'y a qu'</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>un et un seul h1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> sur la page, et qu'il contient le mot-clé ;
+Vérifiez que le contenu est segmenté en plusieurs sous-parties par des h2 et qu'ils contiennent soit le mot-clé, soit un synonyme proche.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Les </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>images ne doivent pas être trop lourdes</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>. Si une image est censée être de petite taille sur le site, il ne faut absolument pas y insérer une grande image et laisser le code faire l'adaptation de taille. En effet, plus l'image est grande, plus elle prend du temps à télécharger.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Vérifiez également que toutes les images contiennent </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>des balises "alt"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> écrites de cette manière : 
+&lt;img src="https://monsite.com/image.png" alt="Description de l'image" /&gt;
+Cette balise sert à expliquer le contenu de l'image aux moteurs de recherche et s'affiche quand les images ne peuvent être chargées. Elle sert aussi à décrire l'image pour les personnes malvoyantes. Il est donc conseillé de décrire correctement l'image et si possible, d'y ajouter le mot-clé.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Il était auparavant conseillé d'écrire un minimum de 250 mots sur une page. De nos jours, il existe très peu de pages en première position avec si peu de contenu. Visez grand </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>minimum 400 mots</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> pour les pages de votre site (lorsque c'est cohérent) et 600 mots pour vos articles de blog, vos pages d'expertise ou d'actualités. </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Vérifier, à l'aide de google analytics,  que l'</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>évolution du trafic</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> va dans le bon sens. En effet, le trafic organique de votre site est censé </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>augmenter</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> ou, au moins, rester </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>stable</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>. Cette étape vous servira également à comprendre sur quels mots-clés votre site remonte avant toute modification SEO. Cela pourra peut-être vous donner des idées de mots-clés que vous auriez oubliés.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Chaque page ne traite que d'</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>un seul sujet,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> c'est à dire qu'elle ne contient qu'un mot clé principal. Ce mot clé doit absolument figurer dans l'URL de la page. Toutes les pages de votre site doivent avoir un seul titre h1, plusieurs h2, au moins 1 image, plusieurs paragaraphe, quelques liens interne et externe. 
+Les pages doivent être liées entre elles de manière cohérente. 
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Plus vous créerez de contenu de qualité, plus vous aurez de pages indexées par Google et donc de </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>portes d'entrées potentielles</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> pour vos visiteurs. Il est donc nécessaire de créer un espace dédié à acceuillir ce contenu. </t>
     </r>
   </si>
 </sst>
@@ -884,7 +996,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -906,12 +1018,6 @@
     </font>
     <font>
       <sz val="12"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -975,13 +1081,25 @@
       <family val="2"/>
     </font>
     <font>
+      <b/>
       <sz val="12"/>
-      <color rgb="FF404040"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="13.5"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Noto Sans"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -992,6 +1110,18 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF7030A0"/>
         <bgColor rgb="FF7030A0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1022,18 +1152,18 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1042,50 +1172,83 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1094,6 +1257,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFDDDDDD"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1303,10 +1471,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z1001"/>
+  <dimension ref="A1:Z1002"/>
   <sheetViews>
-    <sheetView zoomScale="77" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView zoomScale="74" zoomScaleNormal="77" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29:A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1361,344 +1529,562 @@
       <c r="Z1" s="2"/>
     </row>
     <row r="2" spans="1:26" s="6" customFormat="1" ht="104.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" s="6" customFormat="1" ht="147.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="E2" s="4"/>
-    </row>
-    <row r="3" spans="1:26" s="6" customFormat="1" ht="147.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
+      <c r="D3" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="26"/>
+      <c r="F3" s="24" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" s="6" customFormat="1" ht="91.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="4" t="s">
+      <c r="B4" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="8"/>
-    </row>
-    <row r="4" spans="1:26" s="6" customFormat="1" ht="91.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
+      <c r="D4" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="26"/>
+      <c r="F4" s="24"/>
+    </row>
+    <row r="5" spans="1:26" s="6" customFormat="1" ht="108.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="4" t="s">
+      <c r="B5" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="24" t="s">
+        <v>143</v>
+      </c>
+      <c r="D5" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="26"/>
+      <c r="F5" s="24" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" s="25" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" s="8"/>
-    </row>
-    <row r="5" spans="1:26" s="6" customFormat="1" ht="108.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
+      <c r="C6" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="27"/>
+      <c r="E6" s="29"/>
+      <c r="F6" s="27"/>
+    </row>
+    <row r="7" spans="1:26" s="25" customFormat="1" ht="146.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="8"/>
-    </row>
-    <row r="6" spans="1:26" s="6" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
+      <c r="B7" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="27" t="s">
+        <v>144</v>
+      </c>
+      <c r="D7" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="29"/>
+      <c r="F7" s="27"/>
+    </row>
+    <row r="8" spans="1:26" s="6" customFormat="1" ht="146.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="9"/>
-      <c r="E6" s="8"/>
-    </row>
-    <row r="7" spans="1:26" s="6" customFormat="1" ht="146.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
+      <c r="B8" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="C8" s="24" t="s">
+        <v>72</v>
+      </c>
+      <c r="D8" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="E8" s="26"/>
+      <c r="F8" s="24" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" s="25" customFormat="1" ht="146.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="4" t="s">
+      <c r="B9" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="C9" s="27" t="s">
+        <v>145</v>
+      </c>
+      <c r="D9" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="8"/>
-    </row>
-    <row r="8" spans="1:26" s="6" customFormat="1" ht="146.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="E9" s="29"/>
+      <c r="F9" s="27" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" s="6" customFormat="1" ht="146.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="C8" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="E8" s="8"/>
-    </row>
-    <row r="9" spans="1:26" s="6" customFormat="1" ht="146.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
+      <c r="B10" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10" s="26"/>
+      <c r="F10" s="24" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" s="6" customFormat="1" ht="90.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E9" s="8"/>
-    </row>
-    <row r="10" spans="1:26" s="6" customFormat="1" ht="146.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
+      <c r="B11" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="C11" s="24" t="s">
+        <v>146</v>
+      </c>
+      <c r="D11" s="24" t="s">
+        <v>147</v>
+      </c>
+      <c r="E11" s="26"/>
+      <c r="F11" s="24" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" s="6" customFormat="1" ht="90.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B12" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C12" s="24" t="s">
+        <v>148</v>
+      </c>
+      <c r="D12" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="E12" s="26"/>
+      <c r="F12" s="24" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" s="6" customFormat="1" ht="90.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="C13" s="24" t="s">
+        <v>149</v>
+      </c>
+      <c r="D13" s="24" t="s">
+        <v>101</v>
+      </c>
+      <c r="E13" s="26"/>
+      <c r="F13" s="24" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" s="6" customFormat="1" ht="90.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="C14" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="D14" s="24" t="s">
+        <v>104</v>
+      </c>
+      <c r="E14" s="26"/>
+      <c r="F14" s="24" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" s="6" customFormat="1" ht="90.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="E10" s="8"/>
-    </row>
-    <row r="11" spans="1:26" s="6" customFormat="1" ht="90.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
+      <c r="C15" s="24" t="s">
+        <v>150</v>
+      </c>
+      <c r="D15" s="24"/>
+      <c r="E15" s="26"/>
+      <c r="F15" s="24" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" s="6" customFormat="1" ht="147.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B16" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="24" t="s">
+        <v>151</v>
+      </c>
+      <c r="D16" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="E16" s="26"/>
+      <c r="F16" s="24" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" s="6" customFormat="1" ht="147.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="24" t="s">
+        <v>152</v>
+      </c>
+      <c r="D17" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="E17" s="26"/>
+      <c r="F17" s="24" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" s="6" customFormat="1" ht="147.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18" s="24" t="s">
+        <v>153</v>
+      </c>
+      <c r="D18" s="24"/>
+      <c r="E18" s="24"/>
+      <c r="F18" s="24"/>
+    </row>
+    <row r="19" spans="1:6" s="6" customFormat="1" ht="90.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" s="24" t="s">
+        <v>154</v>
+      </c>
+      <c r="D19" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="E19" s="24"/>
+      <c r="F19" s="24" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" s="6" customFormat="1" ht="210.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="D20" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="E20" s="24"/>
+      <c r="F20" s="24" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" s="6" customFormat="1" ht="90.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="33" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="D21" s="24" t="s">
+        <v>155</v>
+      </c>
+      <c r="E21" s="24"/>
+      <c r="F21" s="24"/>
+    </row>
+    <row r="22" spans="1:6" s="6" customFormat="1" ht="90.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="C22" s="24" t="s">
+        <v>156</v>
+      </c>
+      <c r="D22" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="E22" s="24"/>
+      <c r="F22" s="24" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" s="6" customFormat="1" ht="165.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="C23" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="D23" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="E23" s="24"/>
+      <c r="F23" s="24"/>
+    </row>
+    <row r="24" spans="1:6" s="6" customFormat="1" ht="148.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="C24" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="D24" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="C11" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="E11" s="8"/>
-    </row>
-    <row r="12" spans="1:26" s="6" customFormat="1" ht="90.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
+      <c r="E24" s="24"/>
+      <c r="F24" s="24" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" s="15" customFormat="1" ht="90.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="E12" s="8"/>
-    </row>
-    <row r="13" spans="1:26" s="6" customFormat="1" ht="90.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="4" t="s">
+      <c r="B25" s="31" t="s">
+        <v>94</v>
+      </c>
+      <c r="C25" s="31" t="s">
+        <v>93</v>
+      </c>
+      <c r="D25" s="31" t="s">
+        <v>128</v>
+      </c>
+      <c r="E25" s="31"/>
+      <c r="F25" s="31"/>
+    </row>
+    <row r="26" spans="1:6" s="15" customFormat="1" ht="90.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D13" s="9"/>
-      <c r="E13" s="8"/>
-    </row>
-    <row r="14" spans="1:26" s="6" customFormat="1" ht="90.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
+      <c r="B26" s="31" t="s">
+        <v>95</v>
+      </c>
+      <c r="C26" s="31" t="s">
+        <v>96</v>
+      </c>
+      <c r="D26" s="31" t="s">
+        <v>97</v>
+      </c>
+      <c r="E26" s="31"/>
+      <c r="F26" s="31" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" s="6" customFormat="1" ht="90.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="D14" s="9"/>
-      <c r="E14" s="8"/>
-    </row>
-    <row r="15" spans="1:26" s="6" customFormat="1" ht="147.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="4" t="s">
+      <c r="B27" s="24" t="s">
+        <v>98</v>
+      </c>
+      <c r="C27" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="D27" s="24" t="s">
+        <v>100</v>
+      </c>
+      <c r="E27" s="24"/>
+      <c r="F27" s="24" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" s="6" customFormat="1" ht="235.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="B15" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="E15" s="8"/>
-    </row>
-    <row r="16" spans="1:26" s="6" customFormat="1" ht="147.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="4" t="s">
+      <c r="B28" s="24" t="s">
+        <v>109</v>
+      </c>
+      <c r="C28" s="24" t="s">
+        <v>110</v>
+      </c>
+      <c r="D28" s="24" t="s">
+        <v>108</v>
+      </c>
+      <c r="E28" s="24"/>
+      <c r="F28" s="24" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="120.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="B16" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="E16" s="8"/>
-    </row>
-    <row r="17" spans="1:4" s="6" customFormat="1" ht="147.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="4" t="s">
+      <c r="B29" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="C29" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="D29" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="E29" s="24"/>
+      <c r="F29" s="24" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="79.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="B17" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" s="6" customFormat="1" ht="90.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
+      <c r="B30" s="24" t="s">
+        <v>116</v>
+      </c>
+      <c r="C30" s="34" t="s">
+        <v>140</v>
+      </c>
+      <c r="D30" s="24" t="s">
+        <v>141</v>
+      </c>
+      <c r="E30" s="24"/>
+      <c r="F30" s="24" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="B18" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" s="6" customFormat="1" ht="90.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
+      <c r="B31" s="24" t="s">
+        <v>135</v>
+      </c>
+      <c r="C31" s="24" t="s">
+        <v>136</v>
+      </c>
+      <c r="D31" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="E31" s="24"/>
+      <c r="F31" s="24" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="B19" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" s="6" customFormat="1" ht="90.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B20" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" s="6" customFormat="1" ht="90.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B21" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" s="6" customFormat="1" ht="165.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" s="6" customFormat="1" ht="90.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" s="6" customFormat="1" ht="90.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="25" spans="1:4" s="6" customFormat="1" ht="90.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="1:4" s="6" customFormat="1" ht="90.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="1:4" s="6" customFormat="1" ht="90.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="35" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="39" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="40" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="41" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="43" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="44" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="45" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="46" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="47" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="48" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="B32" s="24" t="s">
+        <v>138</v>
+      </c>
+      <c r="C32" s="24" t="s">
+        <v>139</v>
+      </c>
+      <c r="D32" s="24" t="s">
+        <v>142</v>
+      </c>
+      <c r="E32" s="24"/>
+      <c r="F32" s="24"/>
+    </row>
+    <row r="33" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B33" s="13"/>
+      <c r="C33" s="13"/>
+    </row>
+    <row r="34" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B34" s="13"/>
+    </row>
+    <row r="35" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="36" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="37" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="38" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="39" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="40" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="41" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="42" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="43" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="44" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="45" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="46" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="47" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="48" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="49" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="50" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="51" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2652,6 +3038,7 @@
     <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1001" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1002" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup scale="90" fitToWidth="0" fitToHeight="0" orientation="landscape" r:id="rId1"/>
@@ -2662,8 +3049,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="77" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2695,102 +3082,133 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:7" s="19" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="E2" s="18"/>
+      <c r="F2" s="19" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E3" s="10"/>
+      <c r="F3" t="s">
+        <v>113</v>
+      </c>
+      <c r="G3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="198.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E4" s="10"/>
+      <c r="F4" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="150" x14ac:dyDescent="0.2">
+      <c r="A5" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="E5" s="10"/>
+      <c r="F5" t="s">
+        <v>113</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="85.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="B6" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C6" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="D6" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="D2" s="21" t="s">
+      <c r="E6" s="10"/>
+      <c r="F6" t="s">
+        <v>112</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="66.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="B7" s="10" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>82</v>
-      </c>
-      <c r="B3" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="C3" s="21" t="s">
+      <c r="C7" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="87.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="10"/>
+      <c r="B8" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="D3" s="21" t="s">
+      <c r="C8" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="F3" t="s">
-        <v>94</v>
-      </c>
-      <c r="G3" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="31.5" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>82</v>
-      </c>
-      <c r="B4" s="22" t="s">
-        <v>91</v>
-      </c>
-      <c r="C4" s="21" t="s">
-        <v>92</v>
-      </c>
-      <c r="D4" s="21" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>82</v>
-      </c>
-      <c r="B5" t="s">
-        <v>96</v>
-      </c>
-      <c r="C5" t="s">
-        <v>103</v>
-      </c>
-      <c r="D5" s="23" t="s">
-        <v>104</v>
-      </c>
-      <c r="F5" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>82</v>
-      </c>
-      <c r="B6" t="s">
-        <v>98</v>
-      </c>
-      <c r="C6" t="s">
-        <v>99</v>
-      </c>
-      <c r="D6" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>82</v>
-      </c>
-      <c r="B7" t="s">
-        <v>101</v>
-      </c>
-      <c r="C7" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="21" t="s">
-        <v>105</v>
-      </c>
-      <c r="C8" s="21" t="s">
-        <v>106</v>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" t="s">
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -2806,8 +3224,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="72" workbookViewId="0">
-      <selection sqref="A1:F1"/>
+    <sheetView topLeftCell="A3" zoomScale="72" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2817,6 +3235,7 @@
     <col min="3" max="3" width="38.33203125" customWidth="1"/>
     <col min="4" max="4" width="51" customWidth="1"/>
     <col min="5" max="5" width="19.88671875" customWidth="1"/>
+    <col min="7" max="7" width="29.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -2838,80 +3257,95 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="2" spans="1:7" ht="165" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E2" s="4"/>
+      <c r="F2" s="6" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="92.25" x14ac:dyDescent="0.2">
+      <c r="A3" s="10"/>
+      <c r="B3" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="G3" s="10"/>
+    </row>
+    <row r="4" spans="1:7" ht="155.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="10"/>
+      <c r="B4" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E4" s="10"/>
+      <c r="F4" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="G4" s="10"/>
+    </row>
+    <row r="5" spans="1:7" ht="133.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="11"/>
+      <c r="B5" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" s="22" customFormat="1" ht="60" x14ac:dyDescent="0.2">
+      <c r="B6" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C6" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D6" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="E2" s="4"/>
-      <c r="F2" s="6"/>
-    </row>
-    <row r="3" spans="1:7" ht="92.25" x14ac:dyDescent="0.2">
-      <c r="A3" s="13"/>
-      <c r="B3" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-    </row>
-    <row r="4" spans="1:7" ht="155.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="13"/>
-      <c r="B4" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-    </row>
-    <row r="5" spans="1:7" ht="133.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="16"/>
-      <c r="B5" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="C5" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-    </row>
-    <row r="6" spans="1:7" ht="60" x14ac:dyDescent="0.2">
-      <c r="B6" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="C6" s="18" t="s">
-        <v>71</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15" t="s">
+        <v>123</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
enlever style dans html
</commit_message>
<xml_diff>
--- a/annexe/aymeric-audit-SEO.xlsx
+++ b/annexe/aymeric-audit-SEO.xlsx
@@ -19,18 +19,12 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="330"/>
     </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mgajbA1sRpj4h647px0Becg4xhqcQ=="/>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="144">
   <si>
     <t>Catégorie</t>
   </si>
@@ -87,24 +81,6 @@
   </si>
   <si>
     <t xml:space="preserve">Obtenir des citations permet d'augmenter la popularité de votre site. </t>
-  </si>
-  <si>
-    <t>Vérifiez que le site est au moins classé pour le nom de marque</t>
-  </si>
-  <si>
-    <t>Dans la plupart des cas, les sites ayant pour nom de domaine leur nom de marque doivent être placés en 1re place. Si ce n'est pas le cas et que le site n'est pas tout nouveau (créé il y a moins de 3 mois), cela signifie probablement qu'il y a des problèmes d'optimisation SEO.</t>
-  </si>
-  <si>
-    <t>Vérifiez si le site a une version principale (www ou non www)</t>
-  </si>
-  <si>
-    <t>La bonne pratique consiste à choisir l'une des deux puis de rediriger celle qui n'est pas utilisée grâce à une redirection 301.</t>
-  </si>
-  <si>
-    <t>Vérifiez que le site n'a pas de contenu dupliqué</t>
-  </si>
-  <si>
-    <t>Prenez  le temps de vérifier quelques-unes de ces pages à la main. Vous pouvez aussi utiliser un site comme Siteliner, qui repère les problèmes de plagiat automatiquement.</t>
   </si>
   <si>
     <t>Vérifiez les problèmes d'indexation ou de crawling</t>
@@ -408,9 +384,6 @@
     <t>https://markitors.com/keywords-for-seo/</t>
   </si>
   <si>
-    <t>https://www.seo.fr/definition/duplicate-content</t>
-  </si>
-  <si>
     <t>https://www.seo.fr/guide-google-my-business</t>
   </si>
   <si>
@@ -442,12 +415,6 @@
   </si>
   <si>
     <t>Il est très important d'encourager les avis favorables et de répondre aux avis négatifs. Vérifiez sur les plateformes d'avis que vous n'avez pas un compte créé d'office, ce qui est une pratique courante.</t>
-  </si>
-  <si>
-    <t>Une URL de site peut être écrite avec ou sans "www". Ceci n'a pas d'importance au niveau du SEO s'il existe une version principale et qu'elle est bien paramétrée ! Il ne faut surtout pas avoir deux fois le même site en www et sans www</t>
-  </si>
-  <si>
-    <t>Des pages d'un site web ayant du contenu copier-coller ou très similaire sont ce qu'on appelle du "contenu dupliqué". Ce contenu se trouve souvent sur des pages produits similaires ou des pages d'archive ou de catégorie. Il se peut aussi que votre organisation ou client ait copié-collé des pages locales, en ne changeant que le nom de la ville par exemple.</t>
   </si>
   <si>
     <t>Remplacez les URLs impossibles à lire, par exemple "https://monsite.com/345e93", par : "https://monsite.com/mot-cle-principal" !</t>
@@ -589,12 +556,18 @@
   <si>
     <t xml:space="preserve">Ajoutez un élément de focus éléments tel que les liens, les boutons, les images, les formulaires. L'ordre de focus doit être logique. </t>
   </si>
+  <si>
+    <t>https://www.journaldunet.com/solutions/seo-referencement/1490185-comment-referencer-son-site-web-lorsque-l-on-debute-en-seo/</t>
+  </si>
+  <si>
+    <t>Action effectuée</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -657,12 +630,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="13.5"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
@@ -674,7 +641,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -685,18 +652,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF7030A0"/>
         <bgColor rgb="FF7030A0"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -729,7 +684,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -750,16 +705,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -777,29 +723,20 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1022,40 +959,41 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z1000"/>
+  <sheetPr codeName="Feuil1"/>
+  <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="74" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="77" zoomScaleNormal="108" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.77734375" customWidth="1"/>
     <col min="2" max="2" width="23" customWidth="1"/>
-    <col min="3" max="3" width="43.88671875" customWidth="1"/>
+    <col min="3" max="3" width="54" customWidth="1"/>
     <col min="4" max="4" width="49.33203125" customWidth="1"/>
-    <col min="5" max="5" width="65.5546875" customWidth="1"/>
+    <col min="5" max="5" width="36" customWidth="1"/>
     <col min="6" max="6" width="21.33203125" customWidth="1"/>
     <col min="7" max="26" width="10.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="F1" s="14" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="1"/>
@@ -1080,21 +1018,21 @@
       <c r="Z1" s="1"/>
     </row>
     <row r="2" spans="1:26" s="3" customFormat="1" ht="148.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="8" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="E2" s="7"/>
       <c r="F2" s="7" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" spans="1:26" s="3" customFormat="1" ht="147.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1110,9 +1048,9 @@
       <c r="D3" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="9"/>
+      <c r="E3" s="8"/>
       <c r="F3" s="7" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
     </row>
     <row r="4" spans="1:26" s="3" customFormat="1" ht="91.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1128,8 +1066,10 @@
       <c r="D4" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="9"/>
-      <c r="F4" s="7"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="7" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="5" spans="1:26" s="3" customFormat="1" ht="108.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
@@ -1139,668 +1079,675 @@
         <v>10</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="9"/>
+      <c r="E5" s="8"/>
       <c r="F5" s="7" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="6" spans="1:26" s="8" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="10" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" s="3" customFormat="1" ht="146.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" s="3" customFormat="1" ht="146.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C7" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="10"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="10"/>
-    </row>
-    <row r="7" spans="1:26" s="8" customFormat="1" ht="146.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="10" t="s">
+      <c r="D7" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="E7" s="8"/>
+      <c r="F7" s="7" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" s="3" customFormat="1" ht="90.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D8" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" s="3" customFormat="1" ht="121.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" s="3" customFormat="1" ht="90.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" s="3" customFormat="1" ht="90.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" s="3" customFormat="1" ht="90.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="11"/>
-      <c r="F7" s="10"/>
-    </row>
-    <row r="8" spans="1:26" s="3" customFormat="1" ht="146.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="E8" s="9"/>
-      <c r="F8" s="7" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" s="8" customFormat="1" ht="146.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="10" t="s">
+      <c r="C12" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="F12" s="17" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" s="3" customFormat="1" ht="147.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="10" t="s">
-        <v>121</v>
-      </c>
-      <c r="D9" s="10" t="s">
+      <c r="C13" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" s="3" customFormat="1" ht="198.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="B14" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E9" s="11"/>
-      <c r="F9" s="10" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26" s="3" customFormat="1" ht="146.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" s="7" t="s">
+      <c r="C14" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" s="3" customFormat="1" ht="147.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C15" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" s="5" customFormat="1" ht="143.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="C16" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" s="3" customFormat="1" ht="270" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="E10" s="9"/>
-      <c r="F10" s="7" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26" s="3" customFormat="1" ht="90.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="E11" s="9"/>
-      <c r="F11" s="7" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26" s="3" customFormat="1" ht="121.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="E12" s="9"/>
-      <c r="F12" s="7" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26" s="3" customFormat="1" ht="90.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="E13" s="9"/>
-      <c r="F13" s="7" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="14" spans="1:26" s="3" customFormat="1" ht="90.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="E14" s="9"/>
-      <c r="F14" s="7" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="15" spans="1:26" s="3" customFormat="1" ht="90.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B15" s="7" t="s">
+      <c r="C17" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="D17" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="E15" s="9"/>
-      <c r="F15" s="21" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="16" spans="1:26" s="3" customFormat="1" ht="147.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="B16" s="7" t="s">
+      <c r="E17" s="7"/>
+      <c r="F17" s="7" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" s="3" customFormat="1" ht="117" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>148</v>
-      </c>
-      <c r="E16" s="9"/>
-      <c r="F16" s="7" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" s="3" customFormat="1" ht="198.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="12" t="s">
-        <v>133</v>
-      </c>
-      <c r="B17" s="7" t="s">
+      <c r="C18" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="D18" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C17" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="E17" s="9"/>
-      <c r="F17" s="7" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" s="3" customFormat="1" ht="147.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B18" s="7" t="s">
+      <c r="E18" s="7"/>
+      <c r="F18" s="7" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" s="5" customFormat="1" ht="305.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="C18" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-    </row>
-    <row r="19" spans="1:6" s="24" customFormat="1" ht="143.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="B19" s="23" t="s">
+      <c r="C19" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C19" s="22" t="s">
-        <v>126</v>
-      </c>
-      <c r="D19" s="22" t="s">
-        <v>136</v>
-      </c>
-      <c r="E19" s="22"/>
-      <c r="F19" s="22" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" s="3" customFormat="1" ht="257.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="B20" s="19" t="s">
+      <c r="D19" s="9" t="s">
         <v>30</v>
       </c>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" s="3" customFormat="1" ht="148.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>31</v>
+      </c>
       <c r="C20" s="7" t="s">
-        <v>137</v>
+        <v>32</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>31</v>
+        <v>138</v>
       </c>
       <c r="E20" s="7"/>
       <c r="F20" s="7" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" s="5" customFormat="1" ht="90.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="F21" s="9"/>
+    </row>
+    <row r="22" spans="1:6" s="5" customFormat="1" ht="90.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="F22" s="9" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" s="3" customFormat="1" ht="90.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" s="3" customFormat="1" ht="235.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="120.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="79.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="F26" s="7" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="D27" s="7" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" s="3" customFormat="1" ht="117" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B21" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" s="24" customFormat="1" ht="305.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="B22" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="C22" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="D22" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="E22" s="22"/>
-      <c r="F22" s="22"/>
-    </row>
-    <row r="23" spans="1:6" s="3" customFormat="1" ht="148.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" s="5" customFormat="1" ht="90.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="B24" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="C24" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="D24" s="12" t="s">
-        <v>138</v>
-      </c>
-      <c r="E24" s="12"/>
-      <c r="F24" s="12"/>
-    </row>
-    <row r="25" spans="1:6" s="5" customFormat="1" ht="90.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="B25" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="C25" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="D25" s="12" t="s">
-        <v>146</v>
-      </c>
-      <c r="E25" s="12"/>
-      <c r="F25" s="12" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" s="3" customFormat="1" ht="90.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="B26" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="C26" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="D26" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="E26" s="7"/>
-      <c r="F26" s="7" t="s">
+      <c r="E27" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="F27" s="7" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="27" spans="1:6" s="3" customFormat="1" ht="235.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="B27" s="7" t="s">
-        <v>139</v>
-      </c>
-      <c r="C27" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="D27" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="E27" s="7"/>
-      <c r="F27" s="7" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="120.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="12" t="s">
+    <row r="28" spans="1:6" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="9" t="s">
         <v>6</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>86</v>
+        <v>107</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>87</v>
+        <v>108</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>88</v>
+        <v>111</v>
       </c>
       <c r="E28" s="7"/>
       <c r="F28" s="7" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="79.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="B29" s="7" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="163.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="131.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="116.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="F31" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="C29" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="D29" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="E29" s="7"/>
-      <c r="F29" s="7" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="84" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="B30" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="C30" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="D30" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="E30" s="7"/>
-      <c r="F30" s="7" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="84" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="B31" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="C31" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="D31" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="E31" s="7"/>
-      <c r="F31" s="7"/>
-    </row>
-    <row r="32" spans="1:6" ht="141.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="32" spans="1:6" ht="172.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B32" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="C32" s="2" t="s">
+      <c r="B32" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="D32" s="2" t="s">
+      <c r="C32" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="131.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B33" s="2" t="s">
+      <c r="D32" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="E32" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="F32" s="12" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="132" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B33" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C33" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="D33" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="E33" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="F33" s="10" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="188.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E35" s="4"/>
+      <c r="F35" s="4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="145.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="114" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="85.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D38" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="D33" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E33" s="2"/>
-      <c r="F33" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="116.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C34" s="2" t="s">
+      <c r="E38" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="D34" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E34" s="2"/>
-      <c r="F34" s="2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="172.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B35" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="C35" s="16" t="s">
+      <c r="F38" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="150.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="D35" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="E35" s="15"/>
-      <c r="F35" s="15" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" ht="132" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="B36" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="C36" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="D36" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="E36" s="13"/>
-      <c r="F36" s="13" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" ht="84" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="E37" s="4"/>
-      <c r="F37" s="4" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" ht="188.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="E38" s="4"/>
-      <c r="F38" s="4" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" ht="145.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="B39" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="D39" s="6" t="s">
-        <v>72</v>
+      <c r="B39" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>67</v>
       </c>
       <c r="E39" s="4"/>
       <c r="F39" s="4" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" ht="114" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="B40" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D40" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="E40" s="4"/>
-      <c r="F40" s="4" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="85.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="B41" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="C41" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="E41" s="4"/>
-      <c r="F41" s="4" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" ht="150.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="E42" s="4"/>
-      <c r="F42" s="4" t="s">
-        <v>97</v>
-      </c>
-    </row>
+    <row r="40" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="41" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="42" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="43" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="44" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="45" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2756,14 +2703,11 @@
     <row r="995" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="996" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="997" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C35" r:id="rId1" display="https://www.gzip.org/"/>
-    <hyperlink ref="F15" r:id="rId2"/>
-    <hyperlink ref="C36" r:id="rId3" display="http://fr.wikipedia.org/wiki/Lecteur_d%27%C3%A9cran"/>
+    <hyperlink ref="C32" r:id="rId1" display="https://www.gzip.org/"/>
+    <hyperlink ref="F12" r:id="rId2"/>
+    <hyperlink ref="C33" r:id="rId3" display="http://fr.wikipedia.org/wiki/Lecteur_d%27%C3%A9cran"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup scale="90" fitToWidth="0" fitToHeight="0" orientation="landscape" r:id="rId4"/>

</xml_diff>